<commit_message>
Actualizacion final de lista de tareas Rev2
</commit_message>
<xml_diff>
--- a/Lista de tareas individuales/Lista_Tareas_Revision_2_-_David_Barcenas_Duran.xlsx
+++ b/Lista de tareas individuales/Lista_Tareas_Revision_2_-_David_Barcenas_Duran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bestr\Desktop\Repositorios\ItaliaPizza-doc\Lista de tareas individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A82E97-B9D4-4A78-A24B-9A999C738078}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48DC083-8C5B-4DCE-9067-5CB62FE54157}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="80">
   <si>
     <t>Columna</t>
   </si>
@@ -276,7 +276,10 @@
     <t>Codificacion</t>
   </si>
   <si>
-    <t>Por iniciar</t>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Terminado</t>
   </si>
 </sst>
 </file>
@@ -786,11 +789,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AM18" sqref="AM18"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,7 +1094,7 @@
         <v>54</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1185,10 +1188,12 @@
         <f t="shared" ref="AY6:AY10" si="14">AV6-AX6</f>
         <v>4</v>
       </c>
-      <c r="AZ6" s="15"/>
+      <c r="AZ6" s="15">
+        <v>4</v>
+      </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA10" si="15">G6-AZ6</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
@@ -1299,10 +1304,12 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="AZ7" s="15"/>
+      <c r="AZ7" s="15">
+        <v>2.5</v>
+      </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
@@ -1319,7 +1326,7 @@
         <v>54</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
@@ -1413,10 +1420,12 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="AZ8" s="15"/>
+      <c r="AZ8" s="15">
+        <v>4</v>
+      </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
@@ -1433,7 +1442,7 @@
         <v>54</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G9" s="5">
         <v>4</v>
@@ -1527,10 +1536,12 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="AZ9" s="15"/>
+      <c r="AZ9" s="15">
+        <v>2</v>
+      </c>
       <c r="BA9" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
@@ -1547,7 +1558,7 @@
         <v>54</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G10" s="5">
         <v>4</v>
@@ -1641,10 +1652,12 @@
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="AZ10" s="15"/>
+      <c r="AZ10" s="15">
+        <v>4</v>
+      </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
@@ -1661,7 +1674,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G11" s="5">
         <v>4</v>

</xml_diff>

<commit_message>
Actualizacion a lista de tareas
</commit_message>
<xml_diff>
--- a/Lista de tareas individuales/Lista_Tareas_Revision_2_-_David_Barcenas_Duran.xlsx
+++ b/Lista de tareas individuales/Lista_Tareas_Revision_2_-_David_Barcenas_Duran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bestr\Desktop\Repositorios\ItaliaPizza-doc\Lista de tareas individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48DC083-8C5B-4DCE-9067-5CB62FE54157}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DC0454-D6A1-40D6-8CE2-C5EF9890D8FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -790,10 +790,10 @@
   <dimension ref="B1:BA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AG6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="AZ9" sqref="AZ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,11 +1189,11 @@
         <v>4</v>
       </c>
       <c r="AZ6" s="15">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA10" si="15">G6-AZ6</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
@@ -1653,11 +1653,11 @@
         <v>4</v>
       </c>
       <c r="AZ10" s="15">
-        <v>4</v>
+        <v>1.53</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2.4699999999999998</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="43.2" x14ac:dyDescent="0.3">
@@ -1768,14 +1768,21 @@
         <f t="shared" ref="AY11" si="30">AV11-AX11</f>
         <v>4</v>
       </c>
-      <c r="AZ11" s="15"/>
+      <c r="AZ11" s="15">
+        <v>1</v>
+      </c>
       <c r="BA11" s="11">
         <f t="shared" ref="BA11" si="31">G11-AZ11</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -1787,11 +1794,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>